<commit_message>
Resolving failed testcases attached to extent report
</commit_message>
<xml_diff>
--- a/testData/TC_001.xlsx
+++ b/testData/TC_001.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>email</t>
   </si>
@@ -27,9 +27,6 @@
     <t>exp_result</t>
   </si>
   <si>
-    <t>Test123</t>
-  </si>
-  <si>
     <t>valid</t>
   </si>
   <si>
@@ -39,10 +36,13 @@
     <t>lgstester@gmail.com</t>
   </si>
   <si>
-    <t>Test12</t>
-  </si>
-  <si>
     <t>invalid</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>123233</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -438,13 +438,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,21 +452,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated post a job page
</commit_message>
<xml_diff>
--- a/testData/TC_001.xlsx
+++ b/testData/TC_001.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>email</t>
   </si>
@@ -33,16 +33,13 @@
     <t>lgstester50@gmail.com</t>
   </si>
   <si>
-    <t>lgstester@gmail.com</t>
-  </si>
-  <si>
     <t>invalid</t>
   </si>
   <si>
     <t>Test@123</t>
   </si>
   <si>
-    <t>123233</t>
+    <t>Test123</t>
   </si>
 </sst>
 </file>
@@ -415,7 +412,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +438,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -449,13 +446,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>